<commit_message>
aggiornato con dati corretti
</commit_message>
<xml_diff>
--- a/Assignment2/Assignment2.xlsx
+++ b/Assignment2/Assignment2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliam\Desktop\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliam\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABD1FC1-07F3-47FA-87E0-DAEF7E990CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BA74C8-9CF0-43AE-AF37-1F487160F095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VBE" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
   <si>
     <t>Domain</t>
   </si>
@@ -156,9 +156,6 @@
     <t>a-b,b-a</t>
   </si>
   <si>
-    <t>Set di Basic Blocks (nodi)</t>
-  </si>
-  <si>
     <t>Forward</t>
   </si>
   <si>
@@ -242,7 +239,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(x) = Self</t>
+      <t>(x) = Gen</t>
     </r>
     <r>
       <rPr>
@@ -263,12 +260,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> U In[b]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
+      <t xml:space="preserve"> U (Out[x] - Kill</t>
     </r>
     <r>
       <rPr>
@@ -289,7 +281,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(x) = Gen</t>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Coppia di Variabile, Valore</t>
+  </si>
+  <si>
+    <t>in[b] = ^ out[pred(b)]</t>
+  </si>
+  <si>
+    <t>out[b] = ^ in[succ(b)]</t>
+  </si>
+  <si>
+    <r>
+      <t>in[b] = f</t>
     </r>
     <r>
       <rPr>
@@ -310,7 +316,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> U (Out[x] - Kill</t>
+      <t>(out[b])</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>out[b] = f</t>
     </r>
     <r>
       <rPr>
@@ -331,21 +342,76 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Coppia di Variabile, Valore</t>
-  </si>
-  <si>
-    <t>in[b] = ^ out[pred(b)]</t>
-  </si>
-  <si>
-    <t>out[b] = ^ in[succ(b)]</t>
-  </si>
-  <si>
-    <r>
-      <t>in[b] = f</t>
+      <t>(in[b])</t>
+    </r>
+  </si>
+  <si>
+    <t>out[entry] = Ø</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">out[b] = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(k,2)</t>
+  </si>
+  <si>
+    <t>(k,2),(a,4)</t>
+  </si>
+  <si>
+    <t>(k,2),(a,4),(x,5)</t>
+  </si>
+  <si>
+    <t>(k,2),(a,4),(x,8)</t>
+  </si>
+  <si>
+    <t>(a,4)</t>
+  </si>
+  <si>
+    <t>(a,4),(b,2)</t>
+  </si>
+  <si>
+    <t>(a,4),(b,2),(y,8)</t>
+  </si>
+  <si>
+    <t>(k,4),(a,4)</t>
+  </si>
+  <si>
+    <t>(k,4),(a,4),(b,2)</t>
+  </si>
+  <si>
+    <t>Kill = lista di tutte le coppie contenenti la variabile definita nell'istr.</t>
+  </si>
+  <si>
+    <t>Gen = espressione generata</t>
+  </si>
+  <si>
+    <t>Kill = lista di tutte le espressioni contenenti la variabile definita nell'istr.</t>
+  </si>
+  <si>
+    <t>(k,4),(a,4),(b,2),(x,8)</t>
+  </si>
+  <si>
+    <t>(k,4),(a,4),(b,2),(x,8),(y,8)</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
     </r>
     <r>
       <rPr>
@@ -366,12 +432,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(out[b])</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>out[b] = f</t>
+      <t>(x) =  Gen</t>
     </r>
     <r>
       <rPr>
@@ -392,55 +453,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(in[b])</t>
-    </r>
-  </si>
-  <si>
-    <t>out[entry] = Ø</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">out[b] = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>u</t>
-    </r>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>(k,2)</t>
-  </si>
-  <si>
-    <t>(k,2),(a,4)</t>
-  </si>
-  <si>
-    <t>(k,2),(a,4),(x,5)</t>
-  </si>
-  <si>
-    <t>(k,2),(a,4),(x,8)</t>
-  </si>
-  <si>
-    <t>(a,4)</t>
-  </si>
-  <si>
-    <t>(a,4),(b,2)</t>
-  </si>
-  <si>
-    <t>(a,4),(b,2),(y,8)</t>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
+      <t xml:space="preserve"> U (In[x] - Kill</t>
     </r>
     <r>
       <rPr>
@@ -461,7 +474,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(x) = | x - Kill</t>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
     </r>
     <r>
       <rPr>
@@ -482,88 +500,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                     se almeno una variabile non è costante</t>
-    </r>
-  </si>
-  <si>
-    <t>(a,4),(b,2),(x,6),(y,8)</t>
-  </si>
-  <si>
-    <t>(k,4),(a,4)</t>
-  </si>
-  <si>
-    <t>(k,4),(a,4),(b,2)</t>
-  </si>
-  <si>
-    <t>(k,4),(a,4),(b,2),(x,6)</t>
-  </si>
-  <si>
-    <t>(k,4),(a,4),(b,2),(x,6),(y,8)</t>
-  </si>
-  <si>
-    <t>Gen = generazione di coppia Variabile, Valore</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">           | Gen</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> U (x - Kill</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)        se tutte le variabili sono costanti</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">           | x                                 se non sono assegnati valori a variabili</t>
-  </si>
-  <si>
-    <t>Kill = lista di tutte le coppie contenenti la variabile definita nell'istr.</t>
-  </si>
-  <si>
-    <t>Self = il blocco stesso</t>
-  </si>
-  <si>
-    <t>Gen = espressione generata</t>
-  </si>
-  <si>
-    <t>Kill = lista di tutte le espressioni contenenti la variabile definita nell'istr.</t>
+      <t>(x) = b U In[x]</t>
+    </r>
+  </si>
+  <si>
+    <t>Set di Basic Blocks</t>
+  </si>
+  <si>
+    <t>(k,5),(a,4),(b,2),(x,8),(y,8)</t>
+  </si>
+  <si>
+    <t>Gen = generazione di coppia Variabile, Valore (con valori costanti)</t>
   </si>
 </sst>
 </file>
@@ -863,7 +810,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Colore 6" xfId="2" builtinId="50"/>
@@ -994,7 +943,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>157325</xdr:rowOff>
+      <xdr:rowOff>165792</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1300,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1306,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>32</v>
@@ -1366,7 +1315,7 @@
     <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="21"/>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1381,7 +1330,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
@@ -1398,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -1470,17 +1419,17 @@
         <v>31</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1506,7 +1455,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="9" t="s">
@@ -1556,46 +1505,46 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="29"/>
       <c r="B5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
@@ -1603,16 +1552,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1623,13 +1572,13 @@
         <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1637,16 +1586,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O9" s="11"/>
     </row>
@@ -1655,21 +1604,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F10" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1695,17 +1639,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC91B83-FC47-4236-A31F-BE4389B4B074}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1741,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="9" t="s">
@@ -1762,19 +1706,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>31</v>
@@ -1783,7 +1727,7 @@
     <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" s="21"/>
       <c r="B5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1792,169 +1736,167 @@
         <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="B9" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>30</v>
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>62</v>
+      <c r="B11" t="s">
+        <v>81</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>63</v>
+      <c r="B12" t="s">
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1962,16 +1904,16 @@
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1980,43 +1922,37 @@
       <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>81</v>
-      </c>
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -2024,61 +1960,59 @@
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A7:A9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>